<commit_message>
chore: update fix-example-resources pages
</commit_message>
<xml_diff>
--- a/fix-example-resources/StructureDefinition-mii-pr-person-todesursache.xlsx
+++ b/fix-example-resources/StructureDefinition-mii-pr-person-todesursache.xlsx
@@ -992,7 +992,7 @@
 &lt;/valueCoding&gt;</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/sid/icd-10/vs</t>
+    <t>https://www.medizininformatik-initiative.de/fhir/core/modul-person/ValueSet/mii-vs-person-icd10who</t>
   </si>
   <si>
     <t>Condition.code.coding:icd10-who.id</t>
@@ -1877,7 +1877,7 @@
     <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="84.54296875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="48.00390625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="80.39453125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="36.0390625" customWidth="true" bestFit="true"/>

</xml_diff>